<commit_message>
REPORTGEN-566 : add criticity in component REMOVED_VIOLATIONS_LIST
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F598EA-3F6F-4115-B76B-AC4CB71E0447}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5C7FC2-4A79-4683-9486-884760C4552F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="15435" tabRatio="701" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="701" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -675,9 +675,6 @@
   </si>
   <si>
     <t>BCID : name of the BCID to get the rule’s compounded weight and to filter results (60017 by default)</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50</t>
   </si>
   <si>
     <t>* Block Name = AEFP_LIST</t>
@@ -895,6 +892,27 @@
   <si>
     <t>RepGen:TABLE;AETP_LIST;COUNT=-1</t>
   </si>
+  <si>
+    <t>UPDATED</t>
+  </si>
+  <si>
+    <r>
+      <t>CRITICITY =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> c for only critical violations, nc for only non critical violations, all for critical and non critical violations (all by default if not configured)</t>
+    </r>
+  </si>
+  <si>
+    <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50,CRITICITY=all</t>
+  </si>
 </sst>
 </file>
 
@@ -903,7 +921,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1042,6 +1060,21 @@
       <name val="Corbel"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1106,7 +1139,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1180,6 +1213,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1905,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53E83-8DB2-4C9D-B684-50883B392432}">
-  <dimension ref="B1:B8"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,41 +1952,49 @@
     <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="I1" s="31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1975,12 +2018,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -1990,37 +2033,37 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2028,27 +2071,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2073,12 +2116,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2088,17 +2131,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -2111,7 +2154,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2127,7 +2170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822C81FE-2BA1-4A3C-ADB8-F42B4B1305BA}">
   <dimension ref="B1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2139,12 +2182,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2154,7 +2197,7 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -2167,7 +2210,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>